<commit_message>
Separando candidatos de 2018 por gênero
</commit_message>
<xml_diff>
--- a/2018/Norte/AC/relatorioAC.xlsx
+++ b/2018/Norte/AC/relatorioAC.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M253"/>
+  <dimension ref="A1:O253"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,6 +499,16 @@
           <t>Cargo</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>SQ_CANDIDATO</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>DS_GENERO</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -556,6 +566,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N2" t="n">
+        <v>10000600205</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -613,6 +631,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N3" t="n">
+        <v>10000600207</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -670,6 +696,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N4" t="n">
+        <v>10000600209</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -727,6 +761,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N5" t="n">
+        <v>10000600212</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -784,6 +826,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N6" t="n">
+        <v>10000600213</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -841,6 +891,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N7" t="n">
+        <v>10000600214</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -898,6 +956,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N8" t="n">
+        <v>10000600222</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -955,6 +1021,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N9" t="n">
+        <v>10000600230</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1012,6 +1086,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N10" t="n">
+        <v>10000600232</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1069,6 +1151,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N11" t="n">
+        <v>10000600246</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1126,6 +1216,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N12" t="n">
+        <v>10000600839</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1183,6 +1281,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N13" t="n">
+        <v>10000600840</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1240,6 +1346,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N14" t="n">
+        <v>10000600841</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1297,6 +1411,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N15" t="n">
+        <v>10000600842</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1354,6 +1476,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N16" t="n">
+        <v>10000600843</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1411,6 +1541,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N17" t="n">
+        <v>10000600844</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1468,6 +1606,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N18" t="n">
+        <v>10000600845</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1525,6 +1671,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N19" t="n">
+        <v>10000600846</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1582,6 +1736,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N20" t="n">
+        <v>10000600847</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1639,6 +1801,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N21" t="n">
+        <v>10000600848</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1696,6 +1866,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N22" t="n">
+        <v>10000600849</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1753,6 +1931,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N23" t="n">
+        <v>10000600850</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1810,6 +1996,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N24" t="n">
+        <v>10000600851</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1867,6 +2061,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N25" t="n">
+        <v>10000600852</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1924,6 +2126,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N26" t="n">
+        <v>10000600853</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1981,6 +2191,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N27" t="n">
+        <v>10000601164</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2038,6 +2256,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N28" t="n">
+        <v>10000601165</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2095,6 +2321,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N29" t="n">
+        <v>10000601383</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -2152,6 +2386,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N30" t="n">
+        <v>10000602282</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -2209,6 +2451,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N31" t="n">
+        <v>10000602287</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2266,6 +2516,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N32" t="n">
+        <v>10000602288</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2323,6 +2581,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N33" t="n">
+        <v>10000602289</v>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2380,6 +2646,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N34" t="n">
+        <v>10000602290</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2437,6 +2711,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N35" t="n">
+        <v>10000602295</v>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -2494,6 +2776,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N36" t="n">
+        <v>10000602299</v>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2551,6 +2841,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N37" t="n">
+        <v>10000602300</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2608,6 +2906,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N38" t="n">
+        <v>10000602301</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -2665,6 +2971,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N39" t="n">
+        <v>10000602303</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -2722,6 +3036,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N40" t="n">
+        <v>10000602304</v>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -2779,6 +3101,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N41" t="n">
+        <v>10000602305</v>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2836,6 +3166,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N42" t="n">
+        <v>10000602311</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -2893,6 +3231,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N43" t="n">
+        <v>10000602312</v>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2950,6 +3296,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N44" t="n">
+        <v>10000602317</v>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -3007,6 +3361,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N45" t="n">
+        <v>10000602318</v>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -3064,6 +3426,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N46" t="n">
+        <v>10000602508</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -3121,6 +3491,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N47" t="n">
+        <v>10000602509</v>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -3178,6 +3556,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N48" t="n">
+        <v>10000602510</v>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -3235,6 +3621,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N49" t="n">
+        <v>10000602511</v>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -3292,6 +3686,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N50" t="n">
+        <v>10000602512</v>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -3349,6 +3751,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N51" t="n">
+        <v>10000602513</v>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -3406,6 +3816,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N52" t="n">
+        <v>10000602514</v>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -3463,6 +3881,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N53" t="n">
+        <v>10000602515</v>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -3520,6 +3946,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N54" t="n">
+        <v>10000602516</v>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -3577,6 +4011,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N55" t="n">
+        <v>10000602517</v>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -3634,6 +4076,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N56" t="n">
+        <v>10000602518</v>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -3691,6 +4141,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N57" t="n">
+        <v>10000602519</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -3748,6 +4206,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N58" t="n">
+        <v>10000602520</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -3805,6 +4271,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N59" t="n">
+        <v>10000602521</v>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -3862,6 +4336,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N60" t="n">
+        <v>10000602522</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -3919,6 +4401,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N61" t="n">
+        <v>10000602523</v>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -3976,6 +4466,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N62" t="n">
+        <v>10000608398</v>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -4033,6 +4531,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N63" t="n">
+        <v>10000608399</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -4090,6 +4596,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N64" t="n">
+        <v>10000608400</v>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -4147,6 +4661,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N65" t="n">
+        <v>10000608401</v>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -4204,6 +4726,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N66" t="n">
+        <v>10000608402</v>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -4261,6 +4791,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N67" t="n">
+        <v>10000608403</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -4318,6 +4856,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N68" t="n">
+        <v>10000608404</v>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -4375,6 +4921,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N69" t="n">
+        <v>10000608405</v>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -4432,6 +4986,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N70" t="n">
+        <v>10000608406</v>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -4489,6 +5051,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N71" t="n">
+        <v>10000608407</v>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -4546,6 +5116,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N72" t="n">
+        <v>10000608408</v>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -4603,6 +5181,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N73" t="n">
+        <v>10000608409</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -4660,6 +5246,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N74" t="n">
+        <v>10000624630</v>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -4717,6 +5311,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N75" t="n">
+        <v>10000624631</v>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -4774,6 +5376,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N76" t="n">
+        <v>10000624632</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -4831,6 +5441,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N77" t="n">
+        <v>10000624633</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -4888,6 +5506,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N78" t="n">
+        <v>10000624634</v>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -4945,6 +5571,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N79" t="n">
+        <v>10000624635</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -5002,6 +5636,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N80" t="n">
+        <v>10000624636</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -5059,6 +5701,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N81" t="n">
+        <v>10000624637</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -5116,6 +5766,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N82" t="n">
+        <v>10000624638</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -5173,6 +5831,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N83" t="n">
+        <v>10000625359</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -5230,6 +5896,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N84" t="n">
+        <v>10000625360</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -5287,6 +5961,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N85" t="n">
+        <v>10000629579</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -5344,6 +6026,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N86" t="n">
+        <v>10000600205</v>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -5401,6 +6091,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N87" t="n">
+        <v>10000600207</v>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -5458,6 +6156,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N88" t="n">
+        <v>10000600209</v>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -5515,6 +6221,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N89" t="n">
+        <v>10000600212</v>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -5572,6 +6286,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N90" t="n">
+        <v>10000600213</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -5629,6 +6351,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N91" t="n">
+        <v>10000600214</v>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -5686,6 +6416,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N92" t="n">
+        <v>10000600222</v>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -5743,6 +6481,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N93" t="n">
+        <v>10000600230</v>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -5800,6 +6546,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N94" t="n">
+        <v>10000600232</v>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -5857,6 +6611,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N95" t="n">
+        <v>10000600246</v>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -5914,6 +6676,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N96" t="n">
+        <v>10000600839</v>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -5971,6 +6741,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N97" t="n">
+        <v>10000600840</v>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -6028,6 +6806,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N98" t="n">
+        <v>10000600841</v>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -6085,6 +6871,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N99" t="n">
+        <v>10000600842</v>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -6142,6 +6936,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N100" t="n">
+        <v>10000600843</v>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -6199,6 +7001,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N101" t="n">
+        <v>10000600844</v>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -6256,6 +7066,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N102" t="n">
+        <v>10000600845</v>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -6313,6 +7131,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N103" t="n">
+        <v>10000600846</v>
+      </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -6370,6 +7196,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N104" t="n">
+        <v>10000600847</v>
+      </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -6427,6 +7261,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N105" t="n">
+        <v>10000600848</v>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -6484,6 +7326,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N106" t="n">
+        <v>10000600849</v>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -6541,6 +7391,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N107" t="n">
+        <v>10000600850</v>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -6598,6 +7456,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N108" t="n">
+        <v>10000600851</v>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -6655,6 +7521,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N109" t="n">
+        <v>10000600852</v>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -6712,6 +7586,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N110" t="n">
+        <v>10000600853</v>
+      </c>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -6769,6 +7651,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N111" t="n">
+        <v>10000601164</v>
+      </c>
+      <c r="O111" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -6826,6 +7716,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N112" t="n">
+        <v>10000601165</v>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -6883,6 +7781,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N113" t="n">
+        <v>10000601383</v>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -6940,6 +7846,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N114" t="n">
+        <v>10000602282</v>
+      </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -6997,6 +7911,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N115" t="n">
+        <v>10000602287</v>
+      </c>
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -7054,6 +7976,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N116" t="n">
+        <v>10000602288</v>
+      </c>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -7111,6 +8041,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N117" t="n">
+        <v>10000602289</v>
+      </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -7168,6 +8106,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N118" t="n">
+        <v>10000602290</v>
+      </c>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -7225,6 +8171,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N119" t="n">
+        <v>10000602295</v>
+      </c>
+      <c r="O119" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -7282,6 +8236,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N120" t="n">
+        <v>10000602299</v>
+      </c>
+      <c r="O120" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -7339,6 +8301,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N121" t="n">
+        <v>10000602300</v>
+      </c>
+      <c r="O121" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -7396,6 +8366,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N122" t="n">
+        <v>10000602301</v>
+      </c>
+      <c r="O122" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -7453,6 +8431,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N123" t="n">
+        <v>10000602303</v>
+      </c>
+      <c r="O123" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -7510,6 +8496,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N124" t="n">
+        <v>10000602304</v>
+      </c>
+      <c r="O124" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -7567,6 +8561,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N125" t="n">
+        <v>10000602305</v>
+      </c>
+      <c r="O125" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -7624,6 +8626,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N126" t="n">
+        <v>10000602311</v>
+      </c>
+      <c r="O126" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -7681,6 +8691,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N127" t="n">
+        <v>10000602312</v>
+      </c>
+      <c r="O127" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -7738,6 +8756,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N128" t="n">
+        <v>10000602317</v>
+      </c>
+      <c r="O128" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -7795,6 +8821,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N129" t="n">
+        <v>10000602318</v>
+      </c>
+      <c r="O129" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -7852,6 +8886,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N130" t="n">
+        <v>10000602508</v>
+      </c>
+      <c r="O130" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -7909,6 +8951,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N131" t="n">
+        <v>10000602509</v>
+      </c>
+      <c r="O131" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -7966,6 +9016,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N132" t="n">
+        <v>10000602510</v>
+      </c>
+      <c r="O132" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -8023,6 +9081,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N133" t="n">
+        <v>10000602511</v>
+      </c>
+      <c r="O133" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -8080,6 +9146,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N134" t="n">
+        <v>10000602512</v>
+      </c>
+      <c r="O134" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -8137,6 +9211,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N135" t="n">
+        <v>10000602513</v>
+      </c>
+      <c r="O135" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -8194,6 +9276,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N136" t="n">
+        <v>10000602514</v>
+      </c>
+      <c r="O136" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -8251,6 +9341,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N137" t="n">
+        <v>10000602515</v>
+      </c>
+      <c r="O137" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -8308,6 +9406,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N138" t="n">
+        <v>10000602516</v>
+      </c>
+      <c r="O138" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -8365,6 +9471,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N139" t="n">
+        <v>10000602517</v>
+      </c>
+      <c r="O139" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -8422,6 +9536,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N140" t="n">
+        <v>10000602518</v>
+      </c>
+      <c r="O140" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -8479,6 +9601,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N141" t="n">
+        <v>10000602519</v>
+      </c>
+      <c r="O141" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -8536,6 +9666,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N142" t="n">
+        <v>10000602520</v>
+      </c>
+      <c r="O142" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -8593,6 +9731,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N143" t="n">
+        <v>10000602521</v>
+      </c>
+      <c r="O143" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -8650,6 +9796,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N144" t="n">
+        <v>10000602522</v>
+      </c>
+      <c r="O144" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -8707,6 +9861,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N145" t="n">
+        <v>10000602523</v>
+      </c>
+      <c r="O145" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -8764,6 +9926,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N146" t="n">
+        <v>10000608398</v>
+      </c>
+      <c r="O146" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -8821,6 +9991,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N147" t="n">
+        <v>10000608399</v>
+      </c>
+      <c r="O147" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -8878,6 +10056,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N148" t="n">
+        <v>10000608400</v>
+      </c>
+      <c r="O148" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -8935,6 +10121,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N149" t="n">
+        <v>10000608401</v>
+      </c>
+      <c r="O149" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -8992,6 +10186,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N150" t="n">
+        <v>10000608402</v>
+      </c>
+      <c r="O150" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -9049,6 +10251,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N151" t="n">
+        <v>10000608403</v>
+      </c>
+      <c r="O151" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -9106,6 +10316,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N152" t="n">
+        <v>10000608404</v>
+      </c>
+      <c r="O152" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -9163,6 +10381,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N153" t="n">
+        <v>10000608405</v>
+      </c>
+      <c r="O153" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -9220,6 +10446,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N154" t="n">
+        <v>10000608406</v>
+      </c>
+      <c r="O154" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
@@ -9277,6 +10511,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N155" t="n">
+        <v>10000608407</v>
+      </c>
+      <c r="O155" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -9334,6 +10576,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N156" t="n">
+        <v>10000608408</v>
+      </c>
+      <c r="O156" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
@@ -9391,6 +10641,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N157" t="n">
+        <v>10000608409</v>
+      </c>
+      <c r="O157" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -9448,6 +10706,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N158" t="n">
+        <v>10000624630</v>
+      </c>
+      <c r="O158" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
@@ -9505,6 +10771,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N159" t="n">
+        <v>10000624631</v>
+      </c>
+      <c r="O159" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
@@ -9562,6 +10836,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N160" t="n">
+        <v>10000624632</v>
+      </c>
+      <c r="O160" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -9619,6 +10901,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N161" t="n">
+        <v>10000624633</v>
+      </c>
+      <c r="O161" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -9676,6 +10966,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N162" t="n">
+        <v>10000624634</v>
+      </c>
+      <c r="O162" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
@@ -9733,6 +11031,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N163" t="n">
+        <v>10000624635</v>
+      </c>
+      <c r="O163" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -9790,6 +11096,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N164" t="n">
+        <v>10000624636</v>
+      </c>
+      <c r="O164" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -9847,6 +11161,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N165" t="n">
+        <v>10000624637</v>
+      </c>
+      <c r="O165" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -9904,6 +11226,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N166" t="n">
+        <v>10000624638</v>
+      </c>
+      <c r="O166" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
@@ -9961,6 +11291,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N167" t="n">
+        <v>10000625359</v>
+      </c>
+      <c r="O167" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -10018,6 +11356,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N168" t="n">
+        <v>10000625360</v>
+      </c>
+      <c r="O168" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
@@ -10075,6 +11421,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N169" t="n">
+        <v>10000629579</v>
+      </c>
+      <c r="O169" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -10132,6 +11486,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N170" t="n">
+        <v>10000600205</v>
+      </c>
+      <c r="O170" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
@@ -10189,6 +11551,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N171" t="n">
+        <v>10000600207</v>
+      </c>
+      <c r="O171" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
@@ -10246,6 +11616,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N172" t="n">
+        <v>10000600209</v>
+      </c>
+      <c r="O172" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
@@ -10303,6 +11681,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N173" t="n">
+        <v>10000600212</v>
+      </c>
+      <c r="O173" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
@@ -10360,6 +11746,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N174" t="n">
+        <v>10000600213</v>
+      </c>
+      <c r="O174" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
@@ -10417,6 +11811,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N175" t="n">
+        <v>10000600214</v>
+      </c>
+      <c r="O175" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
@@ -10474,6 +11876,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N176" t="n">
+        <v>10000600222</v>
+      </c>
+      <c r="O176" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
@@ -10531,6 +11941,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N177" t="n">
+        <v>10000600230</v>
+      </c>
+      <c r="O177" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
@@ -10588,6 +12006,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N178" t="n">
+        <v>10000600232</v>
+      </c>
+      <c r="O178" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
@@ -10645,6 +12071,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N179" t="n">
+        <v>10000600246</v>
+      </c>
+      <c r="O179" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
@@ -10702,6 +12136,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N180" t="n">
+        <v>10000600839</v>
+      </c>
+      <c r="O180" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
@@ -10759,6 +12201,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N181" t="n">
+        <v>10000600840</v>
+      </c>
+      <c r="O181" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
@@ -10816,6 +12266,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N182" t="n">
+        <v>10000600841</v>
+      </c>
+      <c r="O182" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
@@ -10873,6 +12331,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N183" t="n">
+        <v>10000600842</v>
+      </c>
+      <c r="O183" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
@@ -10930,6 +12396,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N184" t="n">
+        <v>10000600843</v>
+      </c>
+      <c r="O184" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
@@ -10987,6 +12461,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N185" t="n">
+        <v>10000600844</v>
+      </c>
+      <c r="O185" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
@@ -11044,6 +12526,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N186" t="n">
+        <v>10000600845</v>
+      </c>
+      <c r="O186" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
@@ -11101,6 +12591,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N187" t="n">
+        <v>10000600846</v>
+      </c>
+      <c r="O187" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
@@ -11158,6 +12656,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N188" t="n">
+        <v>10000600847</v>
+      </c>
+      <c r="O188" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
@@ -11215,6 +12721,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N189" t="n">
+        <v>10000600848</v>
+      </c>
+      <c r="O189" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
@@ -11272,6 +12786,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N190" t="n">
+        <v>10000600849</v>
+      </c>
+      <c r="O190" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
@@ -11329,6 +12851,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N191" t="n">
+        <v>10000600850</v>
+      </c>
+      <c r="O191" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
@@ -11386,6 +12916,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N192" t="n">
+        <v>10000600851</v>
+      </c>
+      <c r="O192" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
@@ -11443,6 +12981,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N193" t="n">
+        <v>10000600852</v>
+      </c>
+      <c r="O193" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
@@ -11500,6 +13046,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N194" t="n">
+        <v>10000600853</v>
+      </c>
+      <c r="O194" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
@@ -11557,6 +13111,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N195" t="n">
+        <v>10000601164</v>
+      </c>
+      <c r="O195" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
@@ -11614,6 +13176,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N196" t="n">
+        <v>10000601165</v>
+      </c>
+      <c r="O196" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
@@ -11671,6 +13241,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N197" t="n">
+        <v>10000601383</v>
+      </c>
+      <c r="O197" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
@@ -11728,6 +13306,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N198" t="n">
+        <v>10000602282</v>
+      </c>
+      <c r="O198" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
@@ -11785,6 +13371,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N199" t="n">
+        <v>10000602287</v>
+      </c>
+      <c r="O199" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
@@ -11842,6 +13436,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N200" t="n">
+        <v>10000602288</v>
+      </c>
+      <c r="O200" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
@@ -11899,6 +13501,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N201" t="n">
+        <v>10000602289</v>
+      </c>
+      <c r="O201" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
@@ -11956,6 +13566,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N202" t="n">
+        <v>10000602290</v>
+      </c>
+      <c r="O202" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
@@ -12013,6 +13631,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N203" t="n">
+        <v>10000602295</v>
+      </c>
+      <c r="O203" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
@@ -12070,6 +13696,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N204" t="n">
+        <v>10000602299</v>
+      </c>
+      <c r="O204" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
@@ -12127,6 +13761,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N205" t="n">
+        <v>10000602300</v>
+      </c>
+      <c r="O205" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
@@ -12184,6 +13826,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N206" t="n">
+        <v>10000602301</v>
+      </c>
+      <c r="O206" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
@@ -12241,6 +13891,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N207" t="n">
+        <v>10000602303</v>
+      </c>
+      <c r="O207" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
@@ -12298,6 +13956,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N208" t="n">
+        <v>10000602304</v>
+      </c>
+      <c r="O208" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
@@ -12355,6 +14021,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N209" t="n">
+        <v>10000602305</v>
+      </c>
+      <c r="O209" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
@@ -12412,6 +14086,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N210" t="n">
+        <v>10000602311</v>
+      </c>
+      <c r="O210" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
@@ -12469,6 +14151,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N211" t="n">
+        <v>10000602312</v>
+      </c>
+      <c r="O211" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
@@ -12526,6 +14216,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N212" t="n">
+        <v>10000602317</v>
+      </c>
+      <c r="O212" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
@@ -12583,6 +14281,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N213" t="n">
+        <v>10000602318</v>
+      </c>
+      <c r="O213" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
@@ -12640,6 +14346,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N214" t="n">
+        <v>10000602508</v>
+      </c>
+      <c r="O214" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
@@ -12697,6 +14411,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N215" t="n">
+        <v>10000602509</v>
+      </c>
+      <c r="O215" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="n">
@@ -12754,6 +14476,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N216" t="n">
+        <v>10000602510</v>
+      </c>
+      <c r="O216" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="n">
@@ -12811,6 +14541,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N217" t="n">
+        <v>10000602511</v>
+      </c>
+      <c r="O217" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="n">
@@ -12868,6 +14606,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N218" t="n">
+        <v>10000602512</v>
+      </c>
+      <c r="O218" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="n">
@@ -12925,6 +14671,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N219" t="n">
+        <v>10000602513</v>
+      </c>
+      <c r="O219" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
@@ -12982,6 +14736,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N220" t="n">
+        <v>10000602514</v>
+      </c>
+      <c r="O220" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="n">
@@ -13039,6 +14801,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N221" t="n">
+        <v>10000602515</v>
+      </c>
+      <c r="O221" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="n">
@@ -13096,6 +14866,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N222" t="n">
+        <v>10000602516</v>
+      </c>
+      <c r="O222" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
@@ -13153,6 +14931,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N223" t="n">
+        <v>10000602517</v>
+      </c>
+      <c r="O223" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="n">
@@ -13210,6 +14996,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N224" t="n">
+        <v>10000602518</v>
+      </c>
+      <c r="O224" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="n">
@@ -13267,6 +15061,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N225" t="n">
+        <v>10000602519</v>
+      </c>
+      <c r="O225" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
@@ -13324,6 +15126,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N226" t="n">
+        <v>10000602520</v>
+      </c>
+      <c r="O226" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="n">
@@ -13381,6 +15191,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N227" t="n">
+        <v>10000602521</v>
+      </c>
+      <c r="O227" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="n">
@@ -13438,6 +15256,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N228" t="n">
+        <v>10000602522</v>
+      </c>
+      <c r="O228" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="n">
@@ -13495,6 +15321,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N229" t="n">
+        <v>10000602523</v>
+      </c>
+      <c r="O229" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="n">
@@ -13552,6 +15386,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N230" t="n">
+        <v>10000608398</v>
+      </c>
+      <c r="O230" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="n">
@@ -13609,6 +15451,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N231" t="n">
+        <v>10000608399</v>
+      </c>
+      <c r="O231" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="n">
@@ -13666,6 +15516,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N232" t="n">
+        <v>10000608400</v>
+      </c>
+      <c r="O232" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="n">
@@ -13723,6 +15581,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N233" t="n">
+        <v>10000608401</v>
+      </c>
+      <c r="O233" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
@@ -13780,6 +15646,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N234" t="n">
+        <v>10000608402</v>
+      </c>
+      <c r="O234" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="n">
@@ -13837,6 +15711,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N235" t="n">
+        <v>10000608403</v>
+      </c>
+      <c r="O235" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="n">
@@ -13894,6 +15776,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N236" t="n">
+        <v>10000608404</v>
+      </c>
+      <c r="O236" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="n">
@@ -13951,6 +15841,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N237" t="n">
+        <v>10000608405</v>
+      </c>
+      <c r="O237" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="n">
@@ -14008,6 +15906,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N238" t="n">
+        <v>10000608406</v>
+      </c>
+      <c r="O238" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="n">
@@ -14065,6 +15971,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N239" t="n">
+        <v>10000608407</v>
+      </c>
+      <c r="O239" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
@@ -14122,6 +16036,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N240" t="n">
+        <v>10000608408</v>
+      </c>
+      <c r="O240" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="n">
@@ -14179,6 +16101,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N241" t="n">
+        <v>10000608409</v>
+      </c>
+      <c r="O241" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="n">
@@ -14236,6 +16166,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N242" t="n">
+        <v>10000624630</v>
+      </c>
+      <c r="O242" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
@@ -14293,6 +16231,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N243" t="n">
+        <v>10000624631</v>
+      </c>
+      <c r="O243" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
@@ -14350,6 +16296,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N244" t="n">
+        <v>10000624632</v>
+      </c>
+      <c r="O244" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
@@ -14407,6 +16361,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N245" t="n">
+        <v>10000624633</v>
+      </c>
+      <c r="O245" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="n">
@@ -14464,6 +16426,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N246" t="n">
+        <v>10000624634</v>
+      </c>
+      <c r="O246" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="n">
@@ -14521,6 +16491,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N247" t="n">
+        <v>10000624635</v>
+      </c>
+      <c r="O247" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="n">
@@ -14578,6 +16556,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N248" t="n">
+        <v>10000624636</v>
+      </c>
+      <c r="O248" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="n">
@@ -14635,6 +16621,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N249" t="n">
+        <v>10000624637</v>
+      </c>
+      <c r="O249" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="n">
@@ -14692,6 +16686,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N250" t="n">
+        <v>10000624638</v>
+      </c>
+      <c r="O250" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
@@ -14749,6 +16751,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N251" t="n">
+        <v>10000625359</v>
+      </c>
+      <c r="O251" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
@@ -14806,6 +16816,14 @@
           <t>DEPUTADO FEDERAL</t>
         </is>
       </c>
+      <c r="N252" t="n">
+        <v>10000625360</v>
+      </c>
+      <c r="O252" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
@@ -14861,6 +16879,14 @@
       <c r="M253" t="inlineStr">
         <is>
           <t>DEPUTADO FEDERAL</t>
+        </is>
+      </c>
+      <c r="N253" t="n">
+        <v>10000629579</v>
+      </c>
+      <c r="O253" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
         </is>
       </c>
     </row>

</xml_diff>